<commit_message>
adding other indicators sheet
</commit_message>
<xml_diff>
--- a/data/indicators.xlsx
+++ b/data/indicators.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="570" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="560" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Indicators" sheetId="1" r:id="rId1"/>
-    <sheet name="Points" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TrendInd" sheetId="1" r:id="rId1"/>
+    <sheet name="PatternInd" sheetId="4" r:id="rId2"/>
+    <sheet name="CycleInd" sheetId="5" r:id="rId3"/>
+    <sheet name="VolumeInd" sheetId="3" r:id="rId4"/>
+    <sheet name="OverlapInd" sheetId="6" r:id="rId5"/>
+    <sheet name="Points" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511"/>
@@ -443,7 +446,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
@@ -589,11 +592,6 @@
       <sz val="9.0"/>
       <name val="Verdana"/>
       <color rgb="FF00007E"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="맑은 고딕"/>
-      <color theme="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -973,7 +971,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1055,18 +1053,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1075,18 +1061,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1417,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
@@ -1545,11 +1519,6 @@
         <v>29</v>
       </c>
       <c r="G4" s="17"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:12" s="0" customFormat="1" ht="99.000000">
       <c r="A5" s="1" t="s">
@@ -1571,11 +1540,6 @@
       <c r="G5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
-      <c r="K5" s="0"/>
-      <c r="L5" s="0"/>
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" ht="49.500000">
       <c r="A6" s="11" t="s">
@@ -1667,80 +1631,80 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="27" customFormat="1" ht="66.000000">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:12" s="10" customFormat="1" ht="66.000000">
+      <c r="A9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="10">
         <v>24</v>
       </c>
-      <c r="I9" s="27">
-        <v>14</v>
-      </c>
-      <c r="J9" s="27">
-        <v>14</v>
-      </c>
-      <c r="K9" s="27">
-        <v>14</v>
-      </c>
-      <c r="L9" s="27" t="s">
+      <c r="I9" s="10">
+        <v>14</v>
+      </c>
+      <c r="J9" s="10">
+        <v>14</v>
+      </c>
+      <c r="K9" s="10">
+        <v>14</v>
+      </c>
+      <c r="L9" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="27" customFormat="1" ht="82.500000">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:12" s="10" customFormat="1" ht="82.500000">
+      <c r="A10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="10">
         <v>24</v>
       </c>
-      <c r="I10" s="27">
-        <v>14</v>
-      </c>
-      <c r="J10" s="27">
-        <v>14</v>
-      </c>
-      <c r="K10" s="27">
-        <v>14</v>
-      </c>
-      <c r="L10" s="27" t="s">
+      <c r="I10" s="10">
+        <v>14</v>
+      </c>
+      <c r="J10" s="10">
+        <v>14</v>
+      </c>
+      <c r="K10" s="10">
+        <v>14</v>
+      </c>
+      <c r="L10" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="115.500000">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="27" t="s">
         <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1779,7 +1743,7 @@
       <c r="K12" s="0"/>
       <c r="L12" s="0"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" ht="49.500000">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1797,71 +1761,71 @@
       <c r="K13" s="0"/>
       <c r="L13" s="0"/>
     </row>
-    <row r="14" spans="1:12" s="27" customFormat="1" ht="66.000000">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:12" s="10" customFormat="1" ht="66.000000">
+      <c r="A14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="33" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="10">
         <v>24</v>
       </c>
-      <c r="I14" s="27">
-        <v>14</v>
-      </c>
-      <c r="J14" s="27">
-        <v>14</v>
-      </c>
-      <c r="K14" s="27">
-        <v>14</v>
-      </c>
-      <c r="L14" s="27" t="s">
+      <c r="I14" s="10">
+        <v>14</v>
+      </c>
+      <c r="J14" s="10">
+        <v>14</v>
+      </c>
+      <c r="K14" s="10">
+        <v>14</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="34" customFormat="1" ht="49.500000">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:12" s="0" customFormat="1" ht="49.500000">
+      <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="34">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="0">
         <v>24</v>
       </c>
-      <c r="I15" s="34">
-        <v>14</v>
-      </c>
-      <c r="J15" s="34">
-        <v>14</v>
-      </c>
-      <c r="K15" s="34">
-        <v>14</v>
-      </c>
-      <c r="L15" s="34" t="s">
+      <c r="I15" s="0">
+        <v>14</v>
+      </c>
+      <c r="J15" s="0">
+        <v>14</v>
+      </c>
+      <c r="K15" s="0">
+        <v>14</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1903,39 +1867,39 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="27" customFormat="1" ht="82.500000">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:12" s="10" customFormat="1" ht="82.500000">
+      <c r="A20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="10">
         <v>24</v>
       </c>
-      <c r="I20" s="27">
-        <v>14</v>
-      </c>
-      <c r="J20" s="27">
-        <v>14</v>
-      </c>
-      <c r="K20" s="27">
-        <v>14</v>
-      </c>
-      <c r="L20" s="27" t="s">
+      <c r="I20" s="10">
+        <v>14</v>
+      </c>
+      <c r="J20" s="10">
+        <v>14</v>
+      </c>
+      <c r="K20" s="10">
+        <v>14</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1974,233 +1938,233 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="27" customFormat="1" ht="33.000000">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:12" s="10" customFormat="1" ht="33.000000">
+      <c r="A25" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="27">
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="10">
         <v>24</v>
       </c>
-      <c r="I25" s="27">
-        <v>14</v>
-      </c>
-      <c r="J25" s="27">
-        <v>14</v>
-      </c>
-      <c r="K25" s="27">
-        <v>14</v>
-      </c>
-      <c r="L25" s="27" t="s">
+      <c r="I25" s="10">
+        <v>14</v>
+      </c>
+      <c r="J25" s="10">
+        <v>14</v>
+      </c>
+      <c r="K25" s="10">
+        <v>14</v>
+      </c>
+      <c r="L25" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="27" customFormat="1" ht="33.000000">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:12" s="10" customFormat="1" ht="33.000000">
+      <c r="A26" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="27">
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="10">
         <v>24</v>
       </c>
-      <c r="I26" s="27">
-        <v>14</v>
-      </c>
-      <c r="J26" s="27">
-        <v>14</v>
-      </c>
-      <c r="K26" s="27">
-        <v>14</v>
-      </c>
-      <c r="L26" s="27" t="s">
+      <c r="I26" s="10">
+        <v>14</v>
+      </c>
+      <c r="J26" s="10">
+        <v>14</v>
+      </c>
+      <c r="K26" s="10">
+        <v>14</v>
+      </c>
+      <c r="L26" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="27" customFormat="1" ht="33.000000">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:12" s="10" customFormat="1" ht="33.000000">
+      <c r="A27" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="27">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="10">
         <v>24</v>
       </c>
-      <c r="I27" s="27">
-        <v>14</v>
-      </c>
-      <c r="J27" s="27">
-        <v>14</v>
-      </c>
-      <c r="K27" s="27">
-        <v>14</v>
-      </c>
-      <c r="L27" s="27" t="s">
+      <c r="I27" s="10">
+        <v>14</v>
+      </c>
+      <c r="J27" s="10">
+        <v>14</v>
+      </c>
+      <c r="K27" s="10">
+        <v>14</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="27" customFormat="1" ht="56.250000">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:12" s="10" customFormat="1" ht="56.250000">
+      <c r="A28" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="40" t="s">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="10">
         <v>24</v>
       </c>
-      <c r="I28" s="27">
-        <v>14</v>
-      </c>
-      <c r="J28" s="27">
-        <v>14</v>
-      </c>
-      <c r="K28" s="27">
-        <v>14</v>
-      </c>
-      <c r="L28" s="27" t="s">
+      <c r="I28" s="10">
+        <v>14</v>
+      </c>
+      <c r="J28" s="10">
+        <v>14</v>
+      </c>
+      <c r="K28" s="10">
+        <v>14</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="27" customFormat="1" ht="33.000000">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:12" s="10" customFormat="1" ht="33.000000">
+      <c r="A29" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="27">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="10">
         <v>48</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="10">
         <v>28</v>
       </c>
-      <c r="J29" s="27">
+      <c r="J29" s="10">
         <v>28</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K29" s="10">
         <v>28</v>
       </c>
-      <c r="L29" s="27" t="s">
+      <c r="L29" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="27" customFormat="1" ht="66.000000">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:12" s="10" customFormat="1" ht="66.000000">
+      <c r="A30" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28" t="s">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="10">
         <v>12</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="10">
         <v>7</v>
       </c>
-      <c r="J30" s="27">
+      <c r="J30" s="10">
         <v>7</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="10">
         <v>7</v>
       </c>
-      <c r="L30" s="27" t="s">
+      <c r="L30" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="27" customFormat="1" ht="82.500000">
-      <c r="A31" s="28" t="s">
+    <row r="31" spans="1:12" s="10" customFormat="1" ht="82.500000">
+      <c r="A31" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28" t="s">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="10">
         <v>24</v>
       </c>
-      <c r="I31" s="27">
-        <v>14</v>
-      </c>
-      <c r="J31" s="27">
-        <v>14</v>
-      </c>
-      <c r="K31" s="27">
-        <v>14</v>
-      </c>
-      <c r="L31" s="27" t="s">
+      <c r="I31" s="10">
+        <v>14</v>
+      </c>
+      <c r="J31" s="10">
+        <v>14</v>
+      </c>
+      <c r="K31" s="10">
+        <v>14</v>
+      </c>
+      <c r="L31" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2213,63 +2177,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-    </row>
-    <row r="3" spans="1:12" s="26" customFormat="1">
-      <c r="A3" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:L3"/>
-  </mergeCells>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2290,4 +2205,96 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.500000"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.500000"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.500000"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" s="26" customFormat="1">
+      <c r="A3" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:L3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>